<commit_message>
Implement new truncation logic and enhance workbook compilation
- Added logic to truncate data after the first completely empty row in `microplan_compile.py`, improving data handling.
- Updated `compile_microplans_to_workbook` to optionally write cleaned per-project sheets.
- Modified `pipeline_runner.py` to integrate the new compilation functionality, allowing for better organization of micro plan data.
- Updated binary files to reflect changes in the application structure.
</commit_message>
<xml_diff>
--- a/ErectionCompiled_Output_testRun_microplan.xlsx
+++ b/ErectionCompiled_Output_testRun_microplan.xlsx
@@ -880,10 +880,10 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>24301407.98</v>
+        <v>810111</v>
       </c>
       <c r="F16" t="n">
-        <v>2636.355</v>
+        <v>95.69800000000001</v>
       </c>
     </row>
     <row r="17">
@@ -908,10 +908,10 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>35483986.98</v>
+        <v>11992690</v>
       </c>
       <c r="F17" t="n">
-        <v>3832.906</v>
+        <v>1292.249</v>
       </c>
     </row>
     <row r="18">
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1117065</v>
+        <v>1567693</v>
       </c>
       <c r="F19" t="n">
-        <v>126.75</v>
+        <v>180.074</v>
       </c>
     </row>
     <row r="20">
@@ -992,10 +992,10 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>24301407.98</v>
+        <v>359483</v>
       </c>
       <c r="F20" t="n">
-        <v>2636.355</v>
+        <v>42.374</v>
       </c>
     </row>
     <row r="21">
@@ -1076,10 +1076,10 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>2361803</v>
+        <v>1890856</v>
       </c>
       <c r="F23" t="n">
-        <v>263.894</v>
+        <v>208.555</v>
       </c>
     </row>
     <row r="24">
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>828626</v>
+        <v>1299573</v>
       </c>
       <c r="F24" t="n">
-        <v>90.125</v>
+        <v>145.464</v>
       </c>
     </row>
     <row r="25">
@@ -1346,7 +1346,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>

</xml_diff>